<commit_message>
Beginning of minion revamp
- Created a class for managing spawning sequence (no implementation yet)
- Equation for dynamic wave time limit adjusted down
- Wave difficulty equation adjusted up
- Preparing for monsters to have pre-determined stats based on level
- Preparing for monsters to have defined levels, appearing based on difficulty
- Created concept of "value" that determines number to spawn in a wave and gem drop
- Increased attack ranges across the board
- Zombie stats defined
</commit_message>
<xml_diff>
--- a/dev assets/Balancing Tables.xlsx
+++ b/dev assets/Balancing Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxlin\Documents\GitHub\villager-defense-minigame\dev assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D9FD2A-5721-4123-991C-02354BABA38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C715CD-0D34-44E1-9FC1-29DADEAB6695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Health</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Damage Spread</t>
-  </si>
-  <si>
-    <t>Loot</t>
   </si>
   <si>
     <t>Loot Spread</t>
@@ -115,6 +112,12 @@
   </si>
   <si>
     <t>Soldier's Sword</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Custom Multiplier</t>
   </si>
 </sst>
 </file>
@@ -194,6 +197,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Hits to Kill</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -234,7 +262,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$J$1</c:f>
+              <c:f>'Zombie Stats'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -257,44 +285,29 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$J$2:$J$13</c:f>
+              <c:f>'Zombie Stats'!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -312,7 +325,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$K$1</c:f>
+              <c:f>'Zombie Stats'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -335,45 +348,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$K$2:$K$13</c:f>
+              <c:f>'Zombie Stats'!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,7 +388,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$L$1</c:f>
+              <c:f>'Zombie Stats'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -413,10 +411,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$L$2:$L$13</c:f>
+              <c:f>'Zombie Stats'!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -424,34 +422,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,7 +451,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$M$1</c:f>
+              <c:f>'Zombie Stats'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -491,12 +474,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$M$2:$M$13</c:f>
+              <c:f>'Zombie Stats'!$L$2:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -505,31 +488,16 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,7 +514,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$N$1</c:f>
+              <c:f>'Zombie Stats'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -569,15 +537,15 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$N$2:$N$13</c:f>
+              <c:f>'Zombie Stats'!$M$2:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -589,25 +557,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,7 +577,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$O$1</c:f>
+              <c:f>'Zombie Stats'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -649,10 +602,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$O$2:$O$13</c:f>
+              <c:f>'Zombie Stats'!$N$2:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -672,22 +625,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,7 +642,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$P$1</c:f>
+              <c:f>'Zombie Stats'!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -729,10 +667,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$P$2:$P$13</c:f>
+              <c:f>'Zombie Stats'!$O$2:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -752,22 +690,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,7 +707,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$Q$1</c:f>
+              <c:f>'Zombie Stats'!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -809,12 +732,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$Q$2:$Q$13</c:f>
+              <c:f>'Zombie Stats'!$P$2:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -829,25 +752,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,7 +772,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$R$1</c:f>
+              <c:f>'Zombie Stats'!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -889,10 +797,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$R$2:$R$13</c:f>
+              <c:f>'Zombie Stats'!$Q$2:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -900,7 +808,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -913,21 +821,6 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -944,7 +837,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$S$1</c:f>
+              <c:f>'Zombie Stats'!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -969,10 +862,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$S$2:$S$13</c:f>
+              <c:f>'Zombie Stats'!$R$2:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -986,27 +879,12 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1024,7 +902,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$T$1</c:f>
+              <c:f>'Zombie Stats'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1049,10 +927,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$T$2:$T$13</c:f>
+              <c:f>'Zombie Stats'!$S$2:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1073,21 +951,6 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1104,7 +967,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Zombie Stats'!$U$1</c:f>
+              <c:f>'Zombie Stats'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1130,45 +993,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Zombie Stats'!$U$2:$U$13</c:f>
+              <c:f>'Zombie Stats'!$T$2:$T$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1231,13 +1079,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Zombie Stats'!$A$2:$A$13</c15:sqref>
+                          <c15:sqref>'Zombie Stats'!$A$2:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1258,21 +1106,6 @@
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>8</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>9</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>10</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>11</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>12</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2038,16 +1871,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>218590</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>61099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>560724</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>61100</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>125895</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2338,24 +2171,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R17" sqref="R17"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="10" max="19" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2370,7 +2203,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2379,7 +2215,7 @@
         <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>17</v>
@@ -2405,11 +2241,8 @@
       <c r="T1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2417,7 +2250,7 @@
         <v>240</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2426,831 +2259,494 @@
         <v>50</v>
       </c>
       <c r="F2">
-        <f>25*1.15^(A2-1)</f>
-        <v>25</v>
+        <f>(($B2 + 3 * $C2) / 10 / (1 - $D2 * 0.006) + POWER($E2, 1.8) / 50) * $C$14</f>
+        <v>46.865252596366318</v>
+      </c>
+      <c r="I2">
+        <f>IF('Sword Stats'!$E$2 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C2), 0), 100)</f>
+        <v>6</v>
       </c>
       <c r="J2">
-        <f>IF('Sword Stats'!$E$2 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C2), 0), 100)</f>
-        <v>7</v>
+        <f>IF('Sword Stats'!$E$3 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C2), 0), 100)</f>
+        <v>4</v>
       </c>
       <c r="K2">
-        <f>IF('Sword Stats'!$E$3 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C2), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="L2">
         <f>IF('Sword Stats'!$E$4 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C2), 0), 100)</f>
         <v>4</v>
       </c>
+      <c r="L2">
+        <f>IF('Sword Stats'!$E$5 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C2), 0), 100)</f>
+        <v>3</v>
+      </c>
       <c r="M2">
-        <f>IF('Sword Stats'!$E$5 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C2), 0), 100)</f>
-        <v>4</v>
+        <f>IF('Sword Stats'!$E$6 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C2), 0), 100)</f>
+        <v>3</v>
       </c>
       <c r="N2">
-        <f>IF('Sword Stats'!$E$6 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C2), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="O2">
         <f>IF('Sword Stats'!$E$7 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C2), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="P2">
+      <c r="O2">
         <f>IF('Sword Stats'!$E$8 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C2), 0), 100)</f>
         <v>3</v>
       </c>
+      <c r="P2">
+        <f>IF('Sword Stats'!$E$9 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C2), 0), 100)</f>
+        <v>2</v>
+      </c>
       <c r="Q2">
-        <f>IF('Sword Stats'!$E$9 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C2), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="R2">
         <f>IF('Sword Stats'!$E$10 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C2), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="S2">
+      <c r="R2">
         <f>IF('Sword Stats'!$E$11 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C2), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="T2">
+      <c r="S2">
         <f>IF('Sword Stats'!$E$12 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C2), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U2">
+      <c r="T2">
         <f>IF('Sword Stats'!$E$13 - $C2 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C2), 0), 100)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F13" si="0">25*1.15^(A3-1)</f>
-        <v>28.749999999999996</v>
+        <f t="shared" ref="F3:F8" si="0">(($B3 + 3 * $C3) / 10 / (1 - $D3 * 0.006) + POWER($E3, 1.8) / 50) * $C$14</f>
+        <v>68.166886786849503</v>
+      </c>
+      <c r="I3">
+        <f>IF('Sword Stats'!$E$2 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C3), 0), 100)</f>
+        <v>6</v>
       </c>
       <c r="J3">
-        <f>IF('Sword Stats'!$E$2 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C3), 0), 100)</f>
-        <v>8</v>
-      </c>
-      <c r="K3">
         <f>IF('Sword Stats'!$E$3 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C3), 0), 100)</f>
         <v>5</v>
       </c>
-      <c r="L3">
+      <c r="K3">
         <f>IF('Sword Stats'!$E$4 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C3), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="M3">
+      <c r="L3">
         <f>IF('Sword Stats'!$E$5 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C3), 0), 100)</f>
         <v>4</v>
       </c>
+      <c r="M3">
+        <f>IF('Sword Stats'!$E$6 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C3), 0), 100)</f>
+        <v>3</v>
+      </c>
       <c r="N3">
-        <f>IF('Sword Stats'!$E$6 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C3), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="O3">
         <f>IF('Sword Stats'!$E$7 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C3), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="P3">
+      <c r="O3">
         <f>IF('Sword Stats'!$E$8 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C3), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="Q3">
+      <c r="P3">
         <f>IF('Sword Stats'!$E$9 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C3), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="Q3">
         <f>IF('Sword Stats'!$E$10 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C3), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="S3">
+      <c r="R3">
         <f>IF('Sword Stats'!$E$11 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C3), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="T3">
+      <c r="S3">
         <f>IF('Sword Stats'!$E$12 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C3), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U3">
+      <c r="T3">
         <f>IF('Sword Stats'!$E$13 - $C3 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C3), 0), 100)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>280</v>
+        <v>375</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>33.062499999999993</v>
+        <v>87.939518213559367</v>
+      </c>
+      <c r="I4">
+        <f>IF('Sword Stats'!$E$2 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C4), 0), 100)</f>
+        <v>7</v>
       </c>
       <c r="J4">
-        <f>IF('Sword Stats'!$E$2 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C4), 0), 100)</f>
-        <v>10</v>
+        <f>IF('Sword Stats'!$E$3 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C4), 0), 100)</f>
+        <v>5</v>
       </c>
       <c r="K4">
-        <f>IF('Sword Stats'!$E$3 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C4), 0), 100)</f>
-        <v>6</v>
+        <f>IF('Sword Stats'!$E$4 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C4), 0), 100)</f>
+        <v>4</v>
       </c>
       <c r="L4">
-        <f>IF('Sword Stats'!$E$4 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C4), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="M4">
         <f>IF('Sword Stats'!$E$5 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C4), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="N4">
+      <c r="M4">
         <f>IF('Sword Stats'!$E$6 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C4), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="O4">
+      <c r="N4">
         <f>IF('Sword Stats'!$E$7 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C4), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="P4">
+      <c r="O4">
         <f>IF('Sword Stats'!$E$8 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C4), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="Q4">
+      <c r="P4">
         <f>IF('Sword Stats'!$E$9 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C4), 0), 100)</f>
         <v>3</v>
       </c>
+      <c r="Q4">
+        <f>IF('Sword Stats'!$E$10 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C4), 0), 100)</f>
+        <v>2</v>
+      </c>
       <c r="R4">
-        <f>IF('Sword Stats'!$E$10 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C4), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="S4">
         <f>IF('Sword Stats'!$E$11 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C4), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="T4">
+      <c r="S4">
         <f>IF('Sword Stats'!$E$12 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C4), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U4">
+      <c r="T4">
         <f>IF('Sword Stats'!$E$13 - $C4 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C4), 0), 100)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>450</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>38.021874999999987</v>
+        <v>117.48622530959508</v>
+      </c>
+      <c r="I5">
+        <f>IF('Sword Stats'!$E$2 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C5), 0), 100)</f>
+        <v>10</v>
       </c>
       <c r="J5">
-        <f>IF('Sword Stats'!$E$2 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C5), 0), 100)</f>
-        <v>12</v>
+        <f>IF('Sword Stats'!$E$3 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C5), 0), 100)</f>
+        <v>6</v>
       </c>
       <c r="K5">
-        <f>IF('Sword Stats'!$E$3 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C5), 0), 100)</f>
-        <v>7</v>
-      </c>
-      <c r="L5">
         <f>IF('Sword Stats'!$E$4 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C5), 0), 100)</f>
         <v>5</v>
       </c>
+      <c r="L5">
+        <f>IF('Sword Stats'!$E$5 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C5), 0), 100)</f>
+        <v>4</v>
+      </c>
       <c r="M5">
-        <f>IF('Sword Stats'!$E$5 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C5), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="N5">
         <f>IF('Sword Stats'!$E$6 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C5), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="O5">
+      <c r="N5">
         <f>IF('Sword Stats'!$E$7 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C5), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="P5">
+      <c r="O5">
         <f>IF('Sword Stats'!$E$8 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C5), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="Q5">
+      <c r="P5">
         <f>IF('Sword Stats'!$E$9 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C5), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="R5">
+      <c r="Q5">
         <f>IF('Sword Stats'!$E$10 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C5), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="S5">
+      <c r="R5">
         <f>IF('Sword Stats'!$E$11 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C5), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="T5">
+      <c r="S5">
         <f>IF('Sword Stats'!$E$12 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C5), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U5">
+      <c r="T5">
         <f>IF('Sword Stats'!$E$13 - $C5 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C5), 0), 100)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>320</v>
+        <v>500</v>
       </c>
       <c r="C6">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>43.725156249999984</v>
+        <v>141.99256813131808</v>
+      </c>
+      <c r="I6">
+        <f>IF('Sword Stats'!$E$2 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C6), 0), 100)</f>
+        <v>24</v>
       </c>
       <c r="J6">
-        <f>IF('Sword Stats'!$E$2 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C6), 0), 100)</f>
-        <v>16</v>
+        <f>IF('Sword Stats'!$E$3 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C6), 0), 100)</f>
+        <v>9</v>
       </c>
       <c r="K6">
-        <f>IF('Sword Stats'!$E$3 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C6), 0), 100)</f>
-        <v>8</v>
+        <f>IF('Sword Stats'!$E$4 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C6), 0), 100)</f>
+        <v>6</v>
       </c>
       <c r="L6">
-        <f>IF('Sword Stats'!$E$4 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C6), 0), 100)</f>
-        <v>5</v>
+        <f>IF('Sword Stats'!$E$5 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C6), 0), 100)</f>
+        <v>6</v>
       </c>
       <c r="M6">
-        <f>IF('Sword Stats'!$E$5 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C6), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="N6">
         <f>IF('Sword Stats'!$E$6 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C6), 0), 100)</f>
         <v>5</v>
       </c>
-      <c r="O6">
+      <c r="N6">
         <f>IF('Sword Stats'!$E$7 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C6), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="P6">
+      <c r="O6">
         <f>IF('Sword Stats'!$E$8 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C6), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="Q6">
+      <c r="P6">
         <f>IF('Sword Stats'!$E$9 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C6), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="Q6">
         <f>IF('Sword Stats'!$E$10 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C6), 0), 100)</f>
         <v>3</v>
       </c>
+      <c r="R6">
+        <f>IF('Sword Stats'!$E$11 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C6), 0), 100)</f>
+        <v>3</v>
+      </c>
       <c r="S6">
-        <f>IF('Sword Stats'!$E$11 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C6), 0), 100)</f>
-        <v>2</v>
-      </c>
-      <c r="T6">
         <f>IF('Sword Stats'!$E$12 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C6), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U6">
+      <c r="T6">
         <f>IF('Sword Stats'!$E$13 - $C6 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C6), 0), 100)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>340</v>
+        <v>550</v>
       </c>
       <c r="C7">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>50.283929687499985</v>
+        <v>175.26907525086881</v>
+      </c>
+      <c r="I7">
+        <f>IF('Sword Stats'!$E$2 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C7), 0), 100)</f>
+        <v>100</v>
       </c>
       <c r="J7">
-        <f>IF('Sword Stats'!$E$2 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C7), 0), 100)</f>
-        <v>24</v>
+        <f>IF('Sword Stats'!$E$3 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C7), 0), 100)</f>
+        <v>13</v>
       </c>
       <c r="K7">
-        <f>IF('Sword Stats'!$E$3 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C7), 0), 100)</f>
-        <v>9</v>
+        <f>IF('Sword Stats'!$E$4 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C7), 0), 100)</f>
+        <v>8</v>
       </c>
       <c r="L7">
-        <f>IF('Sword Stats'!$E$4 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C7), 0), 100)</f>
+        <f>IF('Sword Stats'!$E$5 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C7), 0), 100)</f>
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <f>IF('Sword Stats'!$E$6 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C7), 0), 100)</f>
         <v>6</v>
       </c>
-      <c r="M7">
-        <f>IF('Sword Stats'!$E$5 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C7), 0), 100)</f>
-        <v>6</v>
-      </c>
       <c r="N7">
-        <f>IF('Sword Stats'!$E$6 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C7), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="O7">
         <f>IF('Sword Stats'!$E$7 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C7), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="P7">
+      <c r="O7">
         <f>IF('Sword Stats'!$E$8 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C7), 0), 100)</f>
         <v>4</v>
       </c>
+      <c r="P7">
+        <f>IF('Sword Stats'!$E$9 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C7), 0), 100)</f>
+        <v>4</v>
+      </c>
       <c r="Q7">
-        <f>IF('Sword Stats'!$E$9 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C7), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="R7">
         <f>IF('Sword Stats'!$E$10 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C7), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="S7">
+      <c r="R7">
         <f>IF('Sword Stats'!$E$11 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C7), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="T7">
+      <c r="S7">
         <f>IF('Sword Stats'!$E$12 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C7), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U7">
+      <c r="T7">
         <f>IF('Sword Stats'!$E$13 - $C7 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C7), 0), 100)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>360</v>
+        <v>650</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E8">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>57.826519140624974</v>
+        <v>206.89045908183044</v>
+      </c>
+      <c r="I8">
+        <f>IF('Sword Stats'!$E$2 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C8), 0), 100)</f>
+        <v>100</v>
       </c>
       <c r="J8">
-        <f>IF('Sword Stats'!$E$2 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C8), 0), 100)</f>
-        <v>48</v>
+        <f>IF('Sword Stats'!$E$3 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C8), 0), 100)</f>
+        <v>18</v>
       </c>
       <c r="K8">
-        <f>IF('Sword Stats'!$E$3 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C8), 0), 100)</f>
-        <v>11</v>
+        <f>IF('Sword Stats'!$E$4 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C8), 0), 100)</f>
+        <v>9</v>
       </c>
       <c r="L8">
-        <f>IF('Sword Stats'!$E$4 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C8), 0), 100)</f>
+        <f>IF('Sword Stats'!$E$5 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C8), 0), 100)</f>
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <f>IF('Sword Stats'!$E$6 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C8), 0), 100)</f>
         <v>7</v>
       </c>
-      <c r="M8">
-        <f>IF('Sword Stats'!$E$5 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C8), 0), 100)</f>
-        <v>6</v>
-      </c>
       <c r="N8">
-        <f>IF('Sword Stats'!$E$6 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C8), 0), 100)</f>
-        <v>6</v>
+        <f>IF('Sword Stats'!$E$7 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C8), 0), 100)</f>
+        <v>5</v>
       </c>
       <c r="O8">
-        <f>IF('Sword Stats'!$E$7 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C8), 0), 100)</f>
+        <f>IF('Sword Stats'!$E$8 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C8), 0), 100)</f>
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <f>IF('Sword Stats'!$E$9 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C8), 0), 100)</f>
         <v>4</v>
       </c>
-      <c r="P8">
-        <f>IF('Sword Stats'!$E$8 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C8), 0), 100)</f>
-        <v>4</v>
-      </c>
       <c r="Q8">
-        <f>IF('Sword Stats'!$E$9 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C8), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="R8">
         <f>IF('Sword Stats'!$E$10 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C8), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="S8">
+      <c r="R8">
         <f>IF('Sword Stats'!$E$11 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C8), 0), 100)</f>
         <v>3</v>
       </c>
-      <c r="T8">
+      <c r="S8">
         <f>IF('Sword Stats'!$E$12 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C8), 0), 100)</f>
         <v>2</v>
       </c>
-      <c r="U8">
+      <c r="T8">
         <f>IF('Sword Stats'!$E$13 - $C8 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C8), 0), 100)</f>
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>380</v>
-      </c>
-      <c r="C9">
-        <v>45</v>
-      </c>
-      <c r="D9">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>85</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>66.500497011718707</v>
-      </c>
-      <c r="J9">
-        <f>IF('Sword Stats'!$E$2 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C9), 0), 100)</f>
-        <v>100</v>
-      </c>
-      <c r="K9">
-        <f>IF('Sword Stats'!$E$3 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C9), 0), 100)</f>
-        <v>13</v>
-      </c>
-      <c r="L9">
-        <f>IF('Sword Stats'!$E$4 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C9), 0), 100)</f>
-        <v>8</v>
-      </c>
-      <c r="M9">
-        <f>IF('Sword Stats'!$E$5 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C9), 0), 100)</f>
-        <v>7</v>
-      </c>
-      <c r="N9">
-        <f>IF('Sword Stats'!$E$6 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C9), 0), 100)</f>
-        <v>6</v>
-      </c>
-      <c r="O9">
-        <f>IF('Sword Stats'!$E$7 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C9), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="P9">
-        <f>IF('Sword Stats'!$E$8 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C9), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="Q9">
-        <f>IF('Sword Stats'!$E$9 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C9), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="R9">
-        <f>IF('Sword Stats'!$E$10 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C9), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="S9">
-        <f>IF('Sword Stats'!$E$11 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C9), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="T9">
-        <f>IF('Sword Stats'!$E$12 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C9), 0), 100)</f>
-        <v>2</v>
-      </c>
-      <c r="U9">
-        <f>IF('Sword Stats'!$E$13 - $C9 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C9), 0), 100)</f>
-        <v>16</v>
+      <c r="C12" s="2">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>400</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>90</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>76.475571563476507</v>
-      </c>
-      <c r="J10">
-        <f>IF('Sword Stats'!$E$2 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C10), 0), 100)</f>
-        <v>100</v>
-      </c>
-      <c r="K10">
-        <f>IF('Sword Stats'!$E$3 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C10), 0), 100)</f>
-        <v>18</v>
-      </c>
-      <c r="L10">
-        <f>IF('Sword Stats'!$E$4 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C10), 0), 100)</f>
-        <v>9</v>
-      </c>
-      <c r="M10">
-        <f>IF('Sword Stats'!$E$5 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C10), 0), 100)</f>
-        <v>8</v>
-      </c>
-      <c r="N10">
-        <f>IF('Sword Stats'!$E$6 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C10), 0), 100)</f>
-        <v>7</v>
-      </c>
-      <c r="O10">
-        <f>IF('Sword Stats'!$E$7 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C10), 0), 100)</f>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="P10">
-        <f>IF('Sword Stats'!$E$8 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C10), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="Q10">
-        <f>IF('Sword Stats'!$E$9 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C10), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="R10">
-        <f>IF('Sword Stats'!$E$10 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C10), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="S10">
-        <f>IF('Sword Stats'!$E$11 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C10), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="T10">
-        <f>IF('Sword Stats'!$E$12 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C10), 0), 100)</f>
-        <v>2</v>
-      </c>
-      <c r="U10">
-        <f>IF('Sword Stats'!$E$13 - $C10 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C10), 0), 100)</f>
-        <v>24</v>
+      <c r="C13" s="2">
+        <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>420</v>
-      </c>
-      <c r="C11">
-        <v>55</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>95</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>87.946907297997981</v>
-      </c>
-      <c r="J11">
-        <f>IF('Sword Stats'!$E$2 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C11), 0), 100)</f>
-        <v>100</v>
-      </c>
-      <c r="K11">
-        <f>IF('Sword Stats'!$E$3 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C11), 0), 100)</f>
-        <v>28</v>
-      </c>
-      <c r="L11">
-        <f>IF('Sword Stats'!$E$4 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C11), 0), 100)</f>
-        <v>11</v>
-      </c>
-      <c r="M11">
-        <f>IF('Sword Stats'!$E$5 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C11), 0), 100)</f>
-        <v>9</v>
-      </c>
-      <c r="N11">
-        <f>IF('Sword Stats'!$E$6 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C11), 0), 100)</f>
-        <v>8</v>
-      </c>
-      <c r="O11">
-        <f>IF('Sword Stats'!$E$7 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C11), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="P11">
-        <f>IF('Sword Stats'!$E$8 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C11), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="Q11">
-        <f>IF('Sword Stats'!$E$9 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C11), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="R11">
-        <f>IF('Sword Stats'!$E$10 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C11), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="S11">
-        <f>IF('Sword Stats'!$E$11 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C11), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="T11">
-        <f>IF('Sword Stats'!$E$12 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C11), 0), 100)</f>
-        <v>2</v>
-      </c>
-      <c r="U11">
-        <f>IF('Sword Stats'!$E$13 - $C11 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C11), 0), 100)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>440</v>
-      </c>
-      <c r="C12">
-        <v>60</v>
-      </c>
-      <c r="D12">
-        <v>16</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>101.13894339269767</v>
-      </c>
-      <c r="J12">
-        <f>IF('Sword Stats'!$E$2 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C12), 0), 100)</f>
-        <v>100</v>
-      </c>
-      <c r="K12">
-        <f>IF('Sword Stats'!$E$3 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C12), 0), 100)</f>
-        <v>64</v>
-      </c>
-      <c r="L12">
-        <f>IF('Sword Stats'!$E$4 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C12), 0), 100)</f>
-        <v>13</v>
-      </c>
-      <c r="M12">
-        <f>IF('Sword Stats'!$E$5 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C12), 0), 100)</f>
-        <v>11</v>
-      </c>
-      <c r="N12">
-        <f>IF('Sword Stats'!$E$6 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C12), 0), 100)</f>
-        <v>10</v>
-      </c>
-      <c r="O12">
-        <f>IF('Sword Stats'!$E$7 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C12), 0), 100)</f>
-        <v>6</v>
-      </c>
-      <c r="P12">
-        <f>IF('Sword Stats'!$E$8 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C12), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="Q12">
-        <f>IF('Sword Stats'!$E$9 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C12), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="R12">
-        <f>IF('Sword Stats'!$E$10 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C12), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="S12">
-        <f>IF('Sword Stats'!$E$11 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C12), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="T12">
-        <f>IF('Sword Stats'!$E$12 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C12), 0), 100)</f>
-        <v>2</v>
-      </c>
-      <c r="U12">
-        <f>IF('Sword Stats'!$E$13 - $C12 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C12), 0), 100)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>460</v>
-      </c>
-      <c r="C13">
-        <v>65</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
-      </c>
-      <c r="E13">
-        <v>105</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>116.30978490160231</v>
-      </c>
-      <c r="J13">
-        <f>IF('Sword Stats'!$E$2 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$2 - $C13), 0), 100)</f>
-        <v>100</v>
-      </c>
-      <c r="K13">
-        <f>IF('Sword Stats'!$E$3 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$3 - $C13), 0), 100)</f>
-        <v>100</v>
-      </c>
-      <c r="L13">
-        <f>IF('Sword Stats'!$E$4 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$4 - $C13), 0), 100)</f>
-        <v>18</v>
-      </c>
-      <c r="M13">
-        <f>IF('Sword Stats'!$E$5 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$5 - $C13), 0), 100)</f>
-        <v>14</v>
-      </c>
-      <c r="N13">
-        <f>IF('Sword Stats'!$E$6 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$6 - $C13), 0), 100)</f>
-        <v>12</v>
-      </c>
-      <c r="O13">
-        <f>IF('Sword Stats'!$E$7 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$7 - $C13), 0), 100)</f>
-        <v>6</v>
-      </c>
-      <c r="P13">
-        <f>IF('Sword Stats'!$E$8 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$8 - $C13), 0), 100)</f>
-        <v>6</v>
-      </c>
-      <c r="Q13">
-        <f>IF('Sword Stats'!$E$9 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$9 - $C13), 0), 100)</f>
-        <v>5</v>
-      </c>
-      <c r="R13">
-        <f>IF('Sword Stats'!$E$10 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$10 - $C13), 0), 100)</f>
-        <v>4</v>
-      </c>
-      <c r="S13">
-        <f>IF('Sword Stats'!$E$11 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$11 - $C13), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="T13">
-        <f>IF('Sword Stats'!$E$12 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$12 - $C13), 0), 100)</f>
-        <v>3</v>
-      </c>
-      <c r="U13">
-        <f>IF('Sword Stats'!$E$13 - $C13 &gt; 0, ROUNDUP(240 / ('Sword Stats'!$E$13 - $C13), 0), 100)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.2</v>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3275,19 +2771,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3501,7 +2997,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>40</v>

</xml_diff>